<commit_message>
tested to make sure things are working and deleted duplicates of data
</commit_message>
<xml_diff>
--- a/Daily Data/OUTPUT/COAL/outages_20241205.xlsx
+++ b/Daily Data/OUTPUT/COAL/outages_20241205.xlsx
@@ -645,16 +645,16 @@
         <v>1465</v>
       </c>
       <c r="E5" s="18" t="n">
-        <v>905</v>
+        <v>1465</v>
       </c>
       <c r="F5" s="18" t="n">
-        <v>905</v>
+        <v>1465</v>
       </c>
       <c r="G5" s="18" t="n">
-        <v>375</v>
+        <v>935</v>
       </c>
       <c r="H5" s="19" t="n">
-        <v>375</v>
+        <v>935</v>
       </c>
     </row>
     <row r="6">
@@ -908,10 +908,10 @@
         <v>66</v>
       </c>
       <c r="G16" s="23" t="n">
-        <v>45635</v>
+        <v>45642</v>
       </c>
       <c r="H16" s="24" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17">
@@ -1111,288 +1111,4 @@
     <firstFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100D001B2BE74D025469E1D0E28F10DD2C8" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3e778ef574344b593b689cacc1c13c14">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="3faa0145-7d03-4bee-a2d8-de479547672d" xmlns:ns3="f69f19e7-36fd-403e-ac68-c4175e96d9c2" xmlns:ns4="d81c2681-db7b-4a56-9abd-a3238a78f6b2" xmlns:ns5="a95247a4-6a6b-40fb-87b6-0fb2f012c536" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bb0fbc2733ec12c07b2f6a837d5cd27e" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="">
-    <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
-    <xsd:import namespace="3faa0145-7d03-4bee-a2d8-de479547672d"/>
-    <xsd:import namespace="f69f19e7-36fd-403e-ac68-c4175e96d9c2"/>
-    <xsd:import namespace="d81c2681-db7b-4a56-9abd-a3238a78f6b2"/>
-    <xsd:import namespace="a95247a4-6a6b-40fb-87b6-0fb2f012c536"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyProperties" minOccurs="0"/>
-                <xsd:element ref="ns1:_ip_UnifiedCompliancePolicyUIAction" minOccurs="0"/>
-                <xsd:element ref="ns4:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns5:TaxCatchAll" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="http://schemas.microsoft.com/sharepoint/v3" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="_ip_UnifiedCompliancePolicyProperties" ma:index="18" nillable="true" ma:displayName="Unified Compliance Policy Properties" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyProperties">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="_ip_UnifiedCompliancePolicyUIAction" ma:index="19" nillable="true" ma:displayName="Unified Compliance Policy UI Action" ma:hidden="true" ma:internalName="_ip_UnifiedCompliancePolicyUIAction">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="3faa0145-7d03-4bee-a2d8-de479547672d" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="10" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="11" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="12" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="13" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceSearchProperties" ma:index="16" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="17" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="f69f19e7-36fd-403e-ac68-c4175e96d9c2" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="14" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="15" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d81c2681-db7b-4a56-9abd-a3238a78f6b2" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="21" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="0c081d5d-8f15-4d39-99f9-175405a35875" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="a95247a4-6a6b-40fb-87b6-0fb2f012c536" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="TaxCatchAll" ma:index="22" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{e56bbf16-6cdf-42b3-a704-f16eb2d403b7}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="a95247a4-6a6b-40fb-87b6-0fb2f012c536">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d81c2681-db7b-4a56-9abd-a3238a78f6b2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a95247a4-6a6b-40fb-87b6-0fb2f012c536" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A64AD48A-0EBF-4448-91D3-6901266E1D97}"/>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5B45C5A3-E2A1-4A59-8844-D43878F2EEE8}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EC34BCD0-35A0-46FB-B69E-5A6B679619DD}"/>
 </file>
</xml_diff>